<commit_message>
(JMT) Updated 1s6, 1s7, 1s11 to meet acceleration specification
</commit_message>
<xml_diff>
--- a/blocks/bl_1s11/bl_1s11.xlsx
+++ b/blocks/bl_1s11/bl_1s11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Foretellix\Files\workspace\AV_ValidationVerification\blocks\bl_1s11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B82F737-2B08-4C05-88E4-C55801277B10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA808C5-BB66-4FC8-9870-3850739A7A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bl_1s6" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>runs</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>[-5..5]m</t>
+  </si>
+  <si>
+    <t>[0..30]kph</t>
+  </si>
+  <si>
+    <t>npc_speed_increase</t>
   </si>
 </sst>
 </file>
@@ -920,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,14 +939,15 @@
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -948,7 +955,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -965,22 +972,25 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -997,18 +1007,21 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
(JMT) Added coverage for bl_1s11 and bl_1s13
</commit_message>
<xml_diff>
--- a/blocks/bl_1s11/bl_1s11.xlsx
+++ b/blocks/bl_1s11/bl_1s11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Foretellix\Files\workspace\AV_ValidationVerification\blocks\bl_1s11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA808C5-BB66-4FC8-9870-3850739A7A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6757FFD-2555-48AD-A3CE-16D51C889BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bl_1s6" sheetId="1" r:id="rId1"/>
@@ -52,18 +52,9 @@
     <t>[70..100]kph</t>
   </si>
   <si>
-    <t>/pub/home/user4/jmt_workspace</t>
-  </si>
-  <si>
-    <t>/pub/home/user4/workshops/msdl_and_foretify/common/workshop_config.sdl</t>
-  </si>
-  <si>
     <t>*bl_1s11</t>
   </si>
   <si>
-    <t>template /pub/home/user4/jmt_workspace/blocks/bl_1s11/bl_1s11.tsdl</t>
-  </si>
-  <si>
     <t>npc_speed_gt_dut_start</t>
   </si>
   <si>
@@ -86,6 +77,15 @@
   </si>
   <si>
     <t>npc_speed_increase</t>
+  </si>
+  <si>
+    <t>/pub/home/user2/jmt_workspace</t>
+  </si>
+  <si>
+    <t>/pub/home/user2/jmt_workspace/workshop_config.sdl</t>
+  </si>
+  <si>
+    <t>template /pub/home/user2/jmt_workspace/blocks/bl_1s11/bl_1s11.tsdl</t>
   </si>
 </sst>
 </file>
@@ -929,7 +929,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,10 +949,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -969,16 +969,16 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
@@ -1004,25 +1004,25 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>